<commit_message>
buggy groub by month
</commit_message>
<xml_diff>
--- a/file/laporanHutang.xlsx
+++ b/file/laporanHutang.xlsx
@@ -358,30 +358,15 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2020-01-01 00:00:00 +0000 UTC</v>
-      </c>
-      <c r="B3" t="str">
-        <v>fery</v>
-      </c>
-      <c r="C3" t="str"/>
-      <c r="D3">
-        <v>5000</v>
-      </c>
-      <c r="E3" t="str">
-        <v>-</v>
-      </c>
-    </row>
-    <row r="4"/>
-    <row r="5">
-      <c r="C5" t="str">
+    <row r="3"/>
+    <row r="4">
+      <c r="C4" t="str">
         <v>Total</v>
       </c>
-      <c r="D5">
-        <v>5000</v>
-      </c>
-      <c r="E5">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>5000</v>
       </c>
     </row>

</xml_diff>